<commit_message>
added variable name, fixed graph labels
</commit_message>
<xml_diff>
--- a/Graphs.xlsx
+++ b/Graphs.xlsx
@@ -380,6 +380,75 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>22</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$C$2:$C$21</c:f>
@@ -460,6 +529,7 @@
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
         <c:crossAx val="108432000"/>
         <c:crosses val="autoZero"/>
@@ -511,7 +581,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
+      <xdr:colOff>428624</xdr:colOff>
       <xdr:row>53</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
@@ -852,8 +922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>